<commit_message>
moved arugement parser to the main section and fixed importing into another python file
</commit_message>
<xml_diff>
--- a/schedule-sample.xlsx
+++ b/schedule-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Sites/badgeserver.onsite/xltozoom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8669DA-BFE7-C74B-A048-521E20A0242B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD21BFE-2CE1-7A43-8BFC-B3123D37BF4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21120" yWindow="8380" windowWidth="28040" windowHeight="17440" xr2:uid="{FC01B0C8-53FD-134D-9529-2A8B38183C2E}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>endtime</t>
   </si>
   <si>
-    <t>eventid</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>timezone</t>
   </si>
   <si>
-    <t>peerreviewid</t>
-  </si>
-  <si>
     <t>meeting_or_webinar</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>zoomid</t>
+  </si>
+  <si>
+    <t>uniqueid</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -461,31 +461,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove debug from create_or_update
</commit_message>
<xml_diff>
--- a/schedule-sample.xlsx
+++ b/schedule-sample.xlsx
@@ -1,142 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Sites/badgeserver.onsite/xltozoom/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C5959-2480-8942-BD1A-A380C52BE856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="22600" yWindow="5460" windowWidth="20920" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15400" windowWidth="21800" xWindow="22600" yWindow="7780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>timezone</t>
-  </si>
-  <si>
-    <t>starttime</t>
-  </si>
-  <si>
-    <t>endtime</t>
-  </si>
-  <si>
-    <t>meeting_or_webinar</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>uniqueid</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>alternative_hosts</t>
-  </si>
-  <si>
-    <t>panelists</t>
-  </si>
-  <si>
-    <t>primarycontact</t>
-  </si>
-  <si>
-    <t>host_zoom_user_email</t>
-  </si>
-  <si>
-    <t>zoomid</t>
-  </si>
-  <si>
-    <t>join_link</t>
-  </si>
-  <si>
-    <t>start_link</t>
-  </si>
-  <si>
-    <t>GMT</t>
-  </si>
-  <si>
-    <t>webinar</t>
-  </si>
-  <si>
-    <t>Lees 2nd test of webinar</t>
-  </si>
-  <si>
-    <t>leewkstest2</t>
-  </si>
-  <si>
-    <t>seaslug</t>
-  </si>
-  <si>
-    <t>example@example.com</t>
-  </si>
-  <si>
-    <t>leetncamp+leewkstest2@gmail.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -152,32 +75,91 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -501,109 +483,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" width="20.83203125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="4" width="17.83203125"/>
+    <col customWidth="1" max="4" min="4" style="4" width="20.33203125"/>
+    <col customWidth="1" max="5" min="5" style="4" width="17.83203125"/>
+    <col customWidth="1" max="7" min="6" width="28.1640625"/>
+    <col customWidth="1" max="8" min="8" width="20.5"/>
+    <col customWidth="1" max="9" min="9" width="26.83203125"/>
+    <col customWidth="1" max="10" min="10" width="20"/>
+    <col customWidth="1" max="11" min="11" width="28.1640625"/>
+    <col customWidth="1" max="12" min="12" width="27.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>timezone</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>starttime</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>endtime</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>meeting_or_webinar</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>uniqueid</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>alternative_hosts</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>panelists</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>primarycontact</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>host_zoom_user_email</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>zoomid</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>join_link</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>start_link</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5">
-        <v>43947.291666666664</v>
-      </c>
-      <c r="D2" s="5">
-        <v>43947.791666666657</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>21</v>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GMT</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>44029.29166666666</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>44029.79166666666</v>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>meeting</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Workshopp Poster Test</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>leewkstest2</t>
+        </is>
+      </c>
+      <c r="I2" s="6" t="inlineStr">
+        <is>
+          <t>example@example.com</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>minivan</t>
+        </is>
+      </c>
+      <c r="L2" s="6" t="inlineStr">
+        <is>
+          <t>leetncamp+leewkstest2@gmail.com</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>82712860401</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>https://us02web.zoom.us/j/82712860401?pwd=VEt0d1R1QTZiT2FlRmZKbWtrMVdoUT09</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>https://us02web.zoom.us/s/82712860401?zak=eyJ6bV9za20iOiJ6bV9vMm0iLCJhbGciOiJIUzI1NiIsInR5cCI6IkpXVCJ9.eyJhdWQiOiJjbGllbnQiLCJ1aWQiOiJkZVNYc1Nna1NYNmV6NnZ5aUhHeXV3IiwiaXNzIjoid2ViIiwic3R5IjoxMDAsIndjZCI6InVzMDIiLCJjbHQiOjAsInN0ayI6ImF5VW4xR08zWFZqbkJxQXM1Z29NQ1Z1aTV6dUZVclhWQzBMTlF3bEJNZHMuQmdVc1puTklWbE5GUlhWT2RGTjRkVEpPSzJSbVpFaFlORVJWWXpGVVoxaDBTSGRWU0haMFVtZHFaa2cxYnoxQU5qWTJaVGN3WlRkalpUWXpaVFkzTUdZellUYzRZbUU1T0RnNE9EQmhOalF4T0dReE4yWm1PV1JpTkdKaVpqWTJaREppT1dJNVptSXdOemMyTXpkbE13QU1NME5DUVhWdmFWbFRNM005QUFSMWN6QXkiLCJleHAiOjE1OTM4MDYyNDcsImlhdCI6MTU5Mzc5OTA0NywiYWlkIjoiSk44N3R2VlVSV0NRdHl0TXNHb25SQSIsImNpZCI6IiJ9.k443LS6X1YfQwKzqd6APFojKFZAgax6Nd0fpUGHHtaY</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{E9030C72-A488-2F4D-BF9A-C6CE06A0353A}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{0503A178-3CF0-6743-BD2D-09DD45123F2F}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved the sample schedule
</commit_message>
<xml_diff>
--- a/schedule-sample.xlsx
+++ b/schedule-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Sites/badgeserver.onsite/xltozoom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B33B0-737E-6C4A-96B5-815288912B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A94AA-D8F3-1740-96CB-EB87A27FDF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22600" yWindow="7780" windowWidth="21800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12880" yWindow="7480" windowWidth="30340" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,18 +67,12 @@
     <t>start_link</t>
   </si>
   <si>
-    <t>GMT</t>
-  </si>
-  <si>
     <t>meeting</t>
   </si>
   <si>
     <t>Workshopp Poster Test</t>
   </si>
   <si>
-    <t>leewkstest2</t>
-  </si>
-  <si>
     <t>example@example.com</t>
   </si>
   <si>
@@ -86,6 +80,12 @@
   </si>
   <si>
     <t>leetncamp+leewkstest2@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>poster-1</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -571,7 +571,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5">
         <v>44029.291666666657</v>
@@ -580,22 +580,22 @@
         <v>44029.791666666657</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>